<commit_message>
:hammer: Add RDS support
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -408,7 +408,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>i-077f867a2d249272b</v>
+        <v>i-xxxxx</v>
       </c>
       <c r="B2" t="str">
         <v>example-instance</v>
@@ -429,6 +429,32 @@
         <v>PePoDev</v>
       </c>
       <c r="H2" t="str">
+        <v>true</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>arn:aws:rds:ap-southeast-1:xxxx:db:simple-db</v>
+      </c>
+      <c r="B3" t="str">
+        <v>simple-db</v>
+      </c>
+      <c r="C3" t="str">
+        <v>RDS</v>
+      </c>
+      <c r="D3" t="str">
+        <v>DB</v>
+      </c>
+      <c r="E3" t="str">
+        <v>ap-southeast-1</v>
+      </c>
+      <c r="F3" t="str">
+        <v>uat</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Moodle</v>
+      </c>
+      <c r="H3" t="str">
         <v>true</v>
       </c>
     </row>

</xml_diff>